<commit_message>
BK's analysis of initial group of papers
</commit_message>
<xml_diff>
--- a/src/maturation_and_reproduction_info.xlsx
+++ b/src/maturation_and_reproduction_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kendall/Box Sync/Home/compadre-plus/src/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Bkendall/Box/Home/compadre-plus/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{5AFA2AE0-65AA-2340-996E-6BC64B7F74A3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CE56D76F-4043-4240-8A6F-95555EF9DDDD}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21540" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{8AAB6499-184D-D44D-A8A6-D26901CF7F3F}"/>
+    <workbookView xWindow="27060" yWindow="460" windowWidth="23760" windowHeight="17440" xr2:uid="{8AAB6499-184D-D44D-A8A6-D26901CF7F3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="125">
   <si>
     <t>doi</t>
   </si>
@@ -301,6 +301,105 @@
   </si>
   <si>
     <t>1-6</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>L1: larval stage | L2: larval stage | L3: larval stage | L4: larval stage | YA: young adult stage</t>
+  </si>
+  <si>
+    <t>9 | 21 | 29 | 37 | 47</t>
+  </si>
+  <si>
+    <t>Stage durations probably represent unmanipulated population. Calculation of gamma based on observed relative growth in length, without explanation</t>
+  </si>
+  <si>
+    <t>3rd larvae</t>
+  </si>
+  <si>
+    <t>1-2</t>
+  </si>
+  <si>
+    <t>2 years is maximimum duration of L3</t>
+  </si>
+  <si>
+    <t>Matrix not presented in paper; original model in months; comadre appears to have applied reported annual hazards to make annual matrix. Critiques are to comadre matrix</t>
+  </si>
+  <si>
+    <t>sub-adults</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Juvenile</t>
+  </si>
+  <si>
+    <t>variable</t>
+  </si>
+  <si>
+    <t>1/T</t>
+  </si>
+  <si>
+    <t>Multiple species with different stage duration. Matrices not shown in paper; comadre doesn't have all the species.</t>
+  </si>
+  <si>
+    <t>Subadult | Adult - no cubs</t>
+  </si>
+  <si>
+    <t>3-7 | var</t>
+  </si>
+  <si>
+    <t>Hatchling and oceanic juvenile | Small juveniles | Large juveniles</t>
+  </si>
+  <si>
+    <t>13 | 10 | 7</t>
+  </si>
+  <si>
+    <t>Open recruitment; stage for size</t>
+  </si>
+  <si>
+    <t>Biological life history not given; transitions based on time-series inversion</t>
+  </si>
+  <si>
+    <t>matrices not in paper; F seems to exclude sex ratio</t>
+  </si>
+  <si>
+    <t>Jueveniles</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>WRONG DOI</t>
+  </si>
+  <si>
+    <t>Tranlation of lower level model to matrix transition not described</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Crouse</t>
+  </si>
+  <si>
+    <t>No models in paper; actual model is in 10.1644/11-MAMM-A-270.1</t>
+  </si>
+  <si>
+    <t>Male juveniles | Male subadults | Female juveniles | Female subadults</t>
+  </si>
+  <si>
+    <t>5 |7 | 16 | 2</t>
+  </si>
+  <si>
+    <t>Caswell 6.103</t>
+  </si>
+  <si>
+    <t>Egg | N1 | N2 | N3 | N4 | N5</t>
+  </si>
+  <si>
+    <t>3.87 | 6.58 | 7.75 | 7.5 | 3.68 | 6.94</t>
   </si>
 </sst>
 </file>
@@ -655,8 +754,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA51811F-8C61-EC46-B5EE-2E716F310EFA}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,7 +768,7 @@
     <col min="3" max="3" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="51" bestFit="1" customWidth="1"/>
   </cols>
@@ -687,7 +789,7 @@
       <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G1" t="s">
@@ -701,16 +803,73 @@
       <c r="A2" t="s">
         <v>49</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H3" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>50</v>
       </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -728,7 +887,7 @@
       <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G5" t="s">
@@ -754,7 +913,7 @@
       <c r="E6" s="1">
         <v>2</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>3</v>
       </c>
       <c r="G6" t="s">
@@ -780,7 +939,7 @@
       <c r="E7" s="1">
         <v>0</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>0</v>
       </c>
       <c r="G7" t="s">
@@ -806,7 +965,7 @@
       <c r="E8" s="1">
         <v>2</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>2</v>
       </c>
       <c r="G8" t="s">
@@ -832,7 +991,7 @@
       <c r="E9" s="1">
         <v>0</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>0</v>
       </c>
       <c r="G9" t="s">
@@ -846,6 +1005,27 @@
       <c r="A10" t="s">
         <v>70</v>
       </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -863,7 +1043,7 @@
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="1">
         <v>0</v>
       </c>
       <c r="G11" t="s">
@@ -889,7 +1069,7 @@
       <c r="E12" s="1">
         <v>0</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="1">
         <v>0</v>
       </c>
       <c r="G12" t="s">
@@ -903,61 +1083,268 @@
       <c r="A13" t="s">
         <v>42</v>
       </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" t="b">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>44</v>
       </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" t="s">
+        <v>83</v>
+      </c>
+      <c r="H14" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="b">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>56</v>
       </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="b">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G16" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>61</v>
       </c>
+      <c r="B17" t="s">
+        <v>77</v>
+      </c>
+      <c r="C17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G17" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>35</v>
       </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G18" t="s">
+        <v>74</v>
+      </c>
+      <c r="H18" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>71</v>
       </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" t="b">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" t="s">
+        <v>74</v>
+      </c>
+      <c r="H19" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>62</v>
       </c>
+      <c r="B20" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G20" t="s">
+        <v>83</v>
+      </c>
+      <c r="H20" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>26</v>
       </c>
+      <c r="H21" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>27</v>
       </c>
+      <c r="H22" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>33</v>
       </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G24" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -968,11 +1355,32 @@
       <c r="A26" t="s">
         <v>48</v>
       </c>
+      <c r="H26" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>22</v>
       </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>72</v>
+      </c>
+      <c r="D27" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
@@ -990,7 +1398,7 @@
       <c r="E28" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="1">
         <v>7</v>
       </c>
       <c r="G28" t="s">
@@ -1004,11 +1412,47 @@
       <c r="A29" t="s">
         <v>36</v>
       </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" t="b">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="G29" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>43</v>
       </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D30" t="b">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G30" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
@@ -1026,7 +1470,7 @@
       <c r="E31" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G31" t="s">
@@ -1037,11 +1481,47 @@
       <c r="A32" t="s">
         <v>69</v>
       </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>46</v>
       </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" t="b">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G33" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
@@ -1109,7 +1589,7 @@
       <c r="E44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G44" t="s">
@@ -1165,7 +1645,7 @@
       <c r="E51" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="1" t="s">
         <v>74</v>
       </c>
       <c r="G51" t="s">
@@ -1191,7 +1671,7 @@
       <c r="E52" s="1">
         <v>0</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="1">
         <v>0</v>
       </c>
       <c r="G52" t="s">

</xml_diff>